<commit_message>
Rate of exciton generation
</commit_message>
<xml_diff>
--- a/solar_simulation_results.xlsx
+++ b/solar_simulation_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,11 @@
           <t># of photons</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Rate of exciton generation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,6 +505,9 @@
       <c r="H2" t="n">
         <v>1.851982751634932e+23</v>
       </c>
+      <c r="I2" t="n">
+        <v>3.703965503269865e+21</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -526,6 +534,9 @@
       <c r="H3" t="n">
         <v>1.855495138997915e+23</v>
       </c>
+      <c r="I3" t="n">
+        <v>3.71099027799583e+21</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -552,6 +563,9 @@
       <c r="H4" t="n">
         <v>1.859297632925714e+23</v>
       </c>
+      <c r="I4" t="n">
+        <v>3.718595265851428e+21</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -578,6 +592,9 @@
       <c r="H5" t="n">
         <v>1.863388086027549e+23</v>
       </c>
+      <c r="I5" t="n">
+        <v>3.726776172055099e+21</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -604,6 +621,9 @@
       <c r="H6" t="n">
         <v>1.867764187491983e+23</v>
       </c>
+      <c r="I6" t="n">
+        <v>3.735528374983967e+21</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -630,6 +650,9 @@
       <c r="H7" t="n">
         <v>1.872423464248102e+23</v>
       </c>
+      <c r="I7" t="n">
+        <v>3.744846928496203e+21</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -655,6 +678,9 @@
       </c>
       <c r="H8" t="n">
         <v>1.877363282221088e+23</v>
+      </c>
+      <c r="I8" t="n">
+        <v>3.754726564442176e+21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CMC started and finished QPA
</commit_message>
<xml_diff>
--- a/solar_simulation_results.xlsx
+++ b/solar_simulation_results.xlsx
@@ -500,13 +500,13 @@
         <v>81371.75177100427</v>
       </c>
       <c r="G2" t="n">
-        <v>73628.20577353852</v>
+        <v>76633.0298535531</v>
       </c>
       <c r="H2" t="n">
-        <v>1.851982751634932e+23</v>
+        <v>2.120319961672114e+23</v>
       </c>
       <c r="I2" t="n">
-        <v>3.703965503269865e+21</v>
+        <v>4.240639923344228e+21</v>
       </c>
     </row>
     <row r="3">
@@ -529,13 +529,13 @@
         <v>81526.07778315095</v>
       </c>
       <c r="G3" t="n">
-        <v>73767.84572390511</v>
+        <v>76778.36861840234</v>
       </c>
       <c r="H3" t="n">
-        <v>1.855495138997915e+23</v>
+        <v>2.124341265343697e+23</v>
       </c>
       <c r="I3" t="n">
-        <v>3.71099027799583e+21</v>
+        <v>4.248682530687393e+21</v>
       </c>
     </row>
     <row r="4">
@@ -558,13 +558,13 @@
         <v>81693.15039315795</v>
       </c>
       <c r="G4" t="n">
-        <v>73919.01927296838</v>
+        <v>76935.71167704028</v>
       </c>
       <c r="H4" t="n">
-        <v>1.859297632925714e+23</v>
+        <v>2.128694709657436e+23</v>
       </c>
       <c r="I4" t="n">
-        <v>3.718595265851428e+21</v>
+        <v>4.257389419314872e+21</v>
       </c>
     </row>
     <row r="5">
@@ -587,13 +587,13 @@
         <v>81872.87524974186</v>
       </c>
       <c r="G5" t="n">
-        <v>74081.64104815664</v>
+        <v>77104.97017277453</v>
       </c>
       <c r="H5" t="n">
-        <v>1.863388086027549e+23</v>
+        <v>2.133377836083127e+23</v>
       </c>
       <c r="I5" t="n">
-        <v>3.726776172055099e+21</v>
+        <v>4.266755672166253e+21</v>
       </c>
     </row>
     <row r="6">
@@ -616,13 +616,13 @@
         <v>82065.15082130121</v>
       </c>
       <c r="G6" t="n">
-        <v>74255.61917987779</v>
+        <v>77286.04848674376</v>
       </c>
       <c r="H6" t="n">
-        <v>1.867764187491983e+23</v>
+        <v>2.138387998991583e+23</v>
       </c>
       <c r="I6" t="n">
-        <v>3.735528374983967e+21</v>
+        <v>4.276775997983167e+21</v>
       </c>
     </row>
     <row r="7">
@@ -645,13 +645,13 @@
         <v>82269.86844693599</v>
       </c>
       <c r="G7" t="n">
-        <v>74440.85534768361</v>
+        <v>77478.84428596617</v>
       </c>
       <c r="H7" t="n">
-        <v>1.872423464248102e+23</v>
+        <v>2.143722366984066e+23</v>
       </c>
       <c r="I7" t="n">
-        <v>3.744846928496203e+21</v>
+        <v>4.287444733968133e+21</v>
       </c>
     </row>
     <row r="8">
@@ -674,13 +674,13 @@
         <v>82486.91239161472</v>
       </c>
       <c r="G8" t="n">
-        <v>74637.24483018706</v>
+        <v>77683.24857529382</v>
       </c>
       <c r="H8" t="n">
-        <v>1.877363282221088e+23</v>
+        <v>2.149377924329784e+23</v>
       </c>
       <c r="I8" t="n">
-        <v>3.754726564442176e+21</v>
+        <v>4.298755848659567e+21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>